<commit_message>
Agregando mas modulos del CPU
</commit_message>
<xml_diff>
--- a/RISC_CPU_Datapath/control unit_example.xlsx
+++ b/RISC_CPU_Datapath/control unit_example.xlsx
@@ -795,13 +795,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -813,18 +819,6 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -834,14 +828,20 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2749,9 +2749,9 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="T19" sqref="T19"/>
+      <pane ySplit="1665" activePane="bottomLeft"/>
+      <selection activeCell="M1" sqref="M1:T1"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,78 +2774,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="29" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="32"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="38"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="O2" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="S2" s="37" t="s">
+      <c r="S2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="37" t="s">
+      <c r="T2" s="23" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3848,11 +3848,10 @@
       <c r="E22" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="M1:T1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="F1:K2"/>
     <mergeCell ref="E1:E2"/>

</xml_diff>